<commit_message>
add summary method: mlp, bilstm, transformer
</commit_message>
<xml_diff>
--- a/CRAN/docs/experiments.xlsx
+++ b/CRAN/docs/experiments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28200" windowHeight="13230" activeTab="1"/>
+    <workbookView windowWidth="27195" windowHeight="12825"/>
   </bookViews>
   <sheets>
     <sheet name="experiments" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="78">
   <si>
     <t>标准参数</t>
   </si>
@@ -108,31 +108,148 @@
     <t>RESULT</t>
   </si>
   <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>params(M)</t>
+  </si>
+  <si>
     <t>valid ppl</t>
   </si>
   <si>
     <t>test ppl</t>
   </si>
   <si>
+    <t>KN5</t>
+  </si>
+  <si>
+    <t>Mikolov &amp; Zweig</t>
+  </si>
+  <si>
+    <t>KN5 + cache</t>
+  </si>
+  <si>
+    <t>RNN</t>
+  </si>
+  <si>
+    <t>RNN-LDA</t>
+  </si>
+  <si>
+    <t>RNN-LDA + KN-5 + cache</t>
+  </si>
+  <si>
+    <t>LSTM (medium)</t>
+  </si>
+  <si>
+    <t>Zaremba</t>
+  </si>
+  <si>
+    <t>LSTM</t>
+  </si>
+  <si>
+    <t>Grave</t>
+  </si>
+  <si>
+    <t>Variational LSTM (medium)</t>
+  </si>
+  <si>
+    <t>Gal &amp; Ghahramani</t>
+  </si>
+  <si>
+    <t>CharCNN</t>
+  </si>
+  <si>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>Variational LSTM (medium, MC)</t>
+  </si>
+  <si>
+    <t>LSTM (large)</t>
+  </si>
+  <si>
+    <t>Variational LSTM (large)</t>
+  </si>
+  <si>
+    <t>Variational LSTM (large, MC)</t>
+  </si>
+  <si>
+    <t>Variational LSTM (tied) + augmented loss</t>
+  </si>
+  <si>
+    <t>Inan</t>
+  </si>
+  <si>
+    <t>LSTM + continuous cache pointer</t>
+  </si>
+  <si>
+    <t>Pointer Sentinel-LSTM</t>
+  </si>
+  <si>
+    <t>Merity</t>
+  </si>
+  <si>
+    <t>Variational RHN (tied)</t>
+  </si>
+  <si>
+    <t>Zilly</t>
+  </si>
+  <si>
+    <t>NAS Cell (tied)</t>
+  </si>
+  <si>
+    <t>Zoph &amp; Le</t>
+  </si>
+  <si>
+    <t>AWD-LSTM</t>
+  </si>
+  <si>
+    <t>Efficient NAS</t>
+  </si>
+  <si>
+    <t>Pham</t>
+  </si>
+  <si>
+    <t>4-layer skip connection LSTM (tied)</t>
+  </si>
+  <si>
+    <t>Melis</t>
+  </si>
+  <si>
+    <t>AWD-LSTM - 3-layer LSTM (tied)</t>
+  </si>
+  <si>
+    <t>Differentiable NAS</t>
+  </si>
+  <si>
+    <t>Liu</t>
+  </si>
+  <si>
+    <t>AWD-LSTM-MoS</t>
+  </si>
+  <si>
+    <t>Yang</t>
+  </si>
+  <si>
+    <t>2-layer skip-LSTM + dropout tuning</t>
+  </si>
+  <si>
     <t>Transformer-XL</t>
   </si>
   <si>
     <t>Dai</t>
   </si>
   <si>
-    <t>AWD-LSTM</t>
-  </si>
-  <si>
-    <t>Merity</t>
-  </si>
-  <si>
-    <t>AWD-LSTM + continuous cache pointer</t>
-  </si>
-  <si>
-    <t>AWD-LSTM-MoS</t>
-  </si>
-  <si>
-    <t>Yang</t>
+    <t>AWD-LSTM-MoS + finetuning</t>
+  </si>
+  <si>
+    <t>AWD-LSTM - 3-layer LSTM (tied) + continuous cache pointer</t>
   </si>
 </sst>
 </file>
@@ -141,9 +258,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -163,7 +280,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -184,30 +309,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -215,37 +318,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -261,17 +334,40 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -284,7 +380,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -297,6 +407,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -307,187 +424,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,11 +618,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -526,21 +682,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -550,21 +691,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -589,156 +715,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1102,8 +1219,8 @@
   <sheetPr/>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1717,96 +1834,604 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="13.25" customWidth="1"/>
+    <col min="1" max="1" width="51.25" customWidth="1"/>
+    <col min="2" max="2" width="17.25" customWidth="1"/>
     <col min="3" max="3" width="13.875" customWidth="1"/>
+    <col min="4" max="4" width="13.125" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:5">
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C2">
+        <v>2012</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>141.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3">
+        <v>2012</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>125.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4">
+        <v>2012</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>124.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5">
+        <v>2012</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>113.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6">
+        <v>2012</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7">
+        <v>2014</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>86.2</v>
+      </c>
+      <c r="F7">
+        <v>82.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>2016</v>
+      </c>
+      <c r="F8">
+        <v>82.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9">
+        <v>2016</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>81.9</v>
+      </c>
+      <c r="F9">
+        <v>79.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10">
+        <v>2016</v>
+      </c>
+      <c r="D10">
+        <v>19</v>
+      </c>
+      <c r="F10">
+        <v>78.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11">
+        <v>2016</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>78.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12">
+        <v>2014</v>
+      </c>
+      <c r="D12">
+        <v>66</v>
+      </c>
+      <c r="E12">
+        <v>82.2</v>
+      </c>
+      <c r="F12">
+        <v>78.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13">
+        <v>2016</v>
+      </c>
+      <c r="D13">
+        <v>66</v>
+      </c>
+      <c r="E13">
+        <v>77.9</v>
+      </c>
+      <c r="F13">
+        <v>75.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14">
+        <v>2016</v>
+      </c>
+      <c r="D14">
+        <v>66</v>
+      </c>
+      <c r="F14">
+        <v>73.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15">
+        <v>2016</v>
+      </c>
+      <c r="D15">
+        <v>24</v>
+      </c>
+      <c r="E15">
+        <v>75.7</v>
+      </c>
+      <c r="F15">
+        <v>73.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16">
+        <v>2016</v>
+      </c>
+      <c r="F16">
+        <v>72.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17">
+        <v>2016</v>
+      </c>
+      <c r="D17">
+        <v>21</v>
+      </c>
+      <c r="E17">
+        <v>72.4</v>
+      </c>
+      <c r="F17">
+        <v>70.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18">
+        <v>2016</v>
+      </c>
+      <c r="D18">
+        <v>51</v>
+      </c>
+      <c r="E18">
+        <v>71.7</v>
+      </c>
+      <c r="F18">
+        <v>68.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19">
+        <v>2016</v>
+      </c>
+      <c r="D19">
+        <v>23</v>
+      </c>
+      <c r="E19">
+        <v>67.9</v>
+      </c>
+      <c r="F19">
+        <v>65.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20">
+        <v>2016</v>
+      </c>
+      <c r="D20">
+        <v>25</v>
+      </c>
+      <c r="F20">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21">
+        <v>2016</v>
+      </c>
+      <c r="D21">
+        <v>54</v>
+      </c>
+      <c r="F21">
+        <v>62.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22">
+        <v>2017</v>
+      </c>
+      <c r="D22">
+        <v>24</v>
+      </c>
+      <c r="E22">
+        <v>60.7</v>
+      </c>
+      <c r="F22">
+        <v>58.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23">
+        <v>2018</v>
+      </c>
+      <c r="D23">
+        <v>24</v>
+      </c>
+      <c r="E23">
+        <v>60.8</v>
+      </c>
+      <c r="F23">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24">
+        <v>2017</v>
+      </c>
+      <c r="D24">
+        <v>24</v>
+      </c>
+      <c r="E24">
+        <v>60.9</v>
+      </c>
+      <c r="F24">
+        <v>58.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25">
+        <v>2017</v>
+      </c>
+      <c r="D25">
+        <v>24</v>
+      </c>
+      <c r="E25">
+        <v>60</v>
+      </c>
+      <c r="F25">
+        <v>57.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26">
+        <v>2018</v>
+      </c>
+      <c r="D26">
+        <v>23</v>
+      </c>
+      <c r="E26">
+        <v>58.3</v>
+      </c>
+      <c r="F26">
+        <v>56.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27">
+        <v>2017</v>
+      </c>
+      <c r="D27">
+        <v>22</v>
+      </c>
+      <c r="E27">
+        <v>58.08</v>
+      </c>
+      <c r="F27">
+        <v>55.97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28">
+        <v>2018</v>
+      </c>
+      <c r="D28">
+        <v>24</v>
+      </c>
+      <c r="E28">
+        <v>57.1</v>
+      </c>
+      <c r="F28">
+        <v>55.3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29">
         <v>2019</v>
       </c>
-      <c r="D2">
+      <c r="D29">
+        <v>24</v>
+      </c>
+      <c r="E29">
         <v>56.72</v>
       </c>
-      <c r="E2">
+      <c r="F29">
         <v>54.52</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3">
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30">
         <v>2017</v>
       </c>
-      <c r="D3">
-        <v>60</v>
-      </c>
-      <c r="E3">
-        <v>57.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4">
+      <c r="D30">
+        <v>22</v>
+      </c>
+      <c r="E30">
+        <v>56.54</v>
+      </c>
+      <c r="F30">
+        <v>54.44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31">
         <v>2017</v>
       </c>
-      <c r="D4">
+      <c r="D31">
+        <v>24</v>
+      </c>
+      <c r="E31">
         <v>53.9</v>
       </c>
-      <c r="E4">
+      <c r="F31">
         <v>52.8</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5">
-        <v>2017</v>
-      </c>
-      <c r="D5">
-        <v>56.54</v>
-      </c>
-      <c r="E5">
-        <v>54.44</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState ref="A2:F33">
+    <sortCondition ref="F2" descending="1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
positional encoding in transformer
</commit_message>
<xml_diff>
--- a/CRAN/docs/experiments.xlsx
+++ b/CRAN/docs/experiments.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27195" windowHeight="12825"/>
+    <workbookView windowWidth="27195" windowHeight="12825" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="experiments" sheetId="1" r:id="rId1"/>
     <sheet name="ptb" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="NL" sheetId="3" r:id="rId3"/>
+    <sheet name="k" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="98">
   <si>
     <t>标准参数</t>
   </si>
@@ -250,6 +251,66 @@
   </si>
   <si>
     <t>AWD-LSTM - 3-layer LSTM (tied) + continuous cache pointer</t>
+  </si>
+  <si>
+    <t>相同覆盖范围下N、L不同取值对模型的影响实验</t>
+  </si>
+  <si>
+    <t>实验名称</t>
+  </si>
+  <si>
+    <t>lowest epoch on</t>
+  </si>
+  <si>
+    <t>time 在不同卡上跑可能没有可比性</t>
+  </si>
+  <si>
+    <t>固定N*L</t>
+  </si>
+  <si>
+    <t>其余参数</t>
+  </si>
+  <si>
+    <t>NL_1</t>
+  </si>
+  <si>
+    <t>2h54m22s</t>
+  </si>
+  <si>
+    <t>NL_2</t>
+  </si>
+  <si>
+    <t>2h57m5s</t>
+  </si>
+  <si>
+    <t>NL_3</t>
+  </si>
+  <si>
+    <t>2h58m39s</t>
+  </si>
+  <si>
+    <t>NL_4</t>
+  </si>
+  <si>
+    <t>2h59m22s</t>
+  </si>
+  <si>
+    <t>NL_5</t>
+  </si>
+  <si>
+    <t>NL_6</t>
+  </si>
+  <si>
+    <t>NL_7</t>
+  </si>
+  <si>
+    <t>NL_8</t>
+  </si>
+  <si>
+    <t>相同N、L取值下，选取zone个数k的影响</t>
+  </si>
+  <si>
+    <t>固定参数</t>
   </si>
 </sst>
 </file>
@@ -257,8 +318,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -271,24 +332,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -302,8 +347,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -317,18 +363,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -342,7 +381,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -351,6 +404,35 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -365,31 +447,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -400,16 +468,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -424,25 +485,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -454,25 +611,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,55 +641,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -544,67 +665,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -615,6 +676,24 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -629,15 +708,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -657,11 +727,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -677,21 +753,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -720,148 +781,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1219,8 +1280,8 @@
   <sheetPr/>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1836,8 +1897,8 @@
   <sheetPr/>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -2441,16 +2502,482 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="H1" sqref="H1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="5" max="5" width="15.875" customWidth="1"/>
+    <col min="6" max="6" width="16.125" customWidth="1"/>
+    <col min="7" max="7" width="14.125" customWidth="1"/>
+    <col min="8" max="8" width="17.375" customWidth="1"/>
+    <col min="9" max="9" width="13.25" customWidth="1"/>
+    <col min="10" max="10" width="19.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>40</v>
+      </c>
+      <c r="H4">
+        <v>25</v>
+      </c>
+      <c r="I4">
+        <v>185.26</v>
+      </c>
+      <c r="J4">
+        <v>177.42</v>
+      </c>
+      <c r="K4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>30</v>
+      </c>
+      <c r="H5">
+        <v>25</v>
+      </c>
+      <c r="I5">
+        <v>188.05</v>
+      </c>
+      <c r="J5">
+        <v>178.42</v>
+      </c>
+      <c r="K5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>24</v>
+      </c>
+      <c r="H6">
+        <v>26</v>
+      </c>
+      <c r="I6">
+        <v>190.92</v>
+      </c>
+      <c r="J6">
+        <v>179.86</v>
+      </c>
+      <c r="K6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>10000</v>
+      </c>
+      <c r="E7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>27</v>
+      </c>
+      <c r="I7">
+        <v>194.82</v>
+      </c>
+      <c r="J7">
+        <v>181.86</v>
+      </c>
+      <c r="K7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>300</v>
+      </c>
+      <c r="E8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8">
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>300</v>
+      </c>
+      <c r="E9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>300</v>
+      </c>
+      <c r="E10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10">
+        <v>20</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11">
+        <v>30</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>0.1</v>
+      </c>
+      <c r="F12">
+        <v>40</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>30</v>
+      </c>
+      <c r="F13">
+        <v>60</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>1111</v>
+      </c>
+      <c r="F14">
+        <v>120</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="17.25" customWidth="1"/>
+    <col min="2" max="2" width="14.375" customWidth="1"/>
+    <col min="7" max="7" width="18.375" customWidth="1"/>
+    <col min="8" max="8" width="12.625" customWidth="1"/>
+    <col min="9" max="9" width="12.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>35</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>10000</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>300</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>300</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>300</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>